<commit_message>
Fill out TaskPlan, add documentation for matlab and simulink, rename matlab files with proper names
</commit_message>
<xml_diff>
--- a/TaskPlan.xlsx
+++ b/TaskPlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregoryseibert/Documents/dhbw-graphische-programmierung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B793E9F-3095-9D4D-8738-BFD92EA9B384}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A31DB-6ED8-EB46-9A0E-4CA919F4C523}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" xr2:uid="{B844A864-B968-094C-9F1D-B9ED8C2FA309}"/>
+    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16180" xr2:uid="{B844A864-B968-094C-9F1D-B9ED8C2FA309}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -102,7 +102,10 @@
     <t>Standard Error</t>
   </si>
   <si>
-    <t>Actual Case</t>
+    <t>Actual Project Time (in h)</t>
+  </si>
+  <si>
+    <t>Actual Time</t>
   </si>
 </sst>
 </file>
@@ -678,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E6F04A-8579-EA48-AC2A-F124B89258CD}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,7 +720,7 @@
         <v>22</v>
       </c>
       <c r="J1" s="17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -735,11 +738,11 @@
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="4">
-        <f t="shared" ref="F2:F12" si="0">(B2+4*C2+D2)/6</f>
+        <f>(B2+4*C2+D2)/6</f>
         <v>10</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" ref="G2:G12" si="1">(D2-B2)/6</f>
+        <f t="shared" ref="G2:G12" si="0">(D2-B2)/6</f>
         <v>1.6666666666666667</v>
       </c>
       <c r="H2" s="4">
@@ -765,11 +768,11 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="3">
+        <f t="shared" ref="F2:F12" si="1">(B3+4*C3+D3)/6</f>
+        <v>45</v>
+      </c>
+      <c r="G3" s="16">
         <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="G3" s="16">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H3" s="3">
@@ -795,11 +798,11 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="3">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G4" s="16">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G4" s="16">
-        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="H4" s="3">
@@ -825,11 +828,11 @@
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="G5" s="16">
-        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="H5" s="3">
@@ -855,11 +858,11 @@
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G6" s="16">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G6" s="16">
-        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="H6" s="3">
@@ -885,11 +888,11 @@
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="3">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="G7" s="16">
         <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="G7" s="16">
-        <f t="shared" si="1"/>
         <v>3.3333333333333335</v>
       </c>
       <c r="H7" s="3">
@@ -915,18 +918,20 @@
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="3">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="G8" s="16">
         <f t="shared" si="0"/>
-        <v>90</v>
-      </c>
-      <c r="G8" s="16">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H8" s="3">
         <f t="shared" si="2"/>
         <v>1.507556722888818</v>
       </c>
-      <c r="J8" s="3"/>
+      <c r="J8" s="3">
+        <v>100</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -943,18 +948,20 @@
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="3">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="G9" s="16">
         <f t="shared" si="0"/>
-        <v>75</v>
-      </c>
-      <c r="G9" s="16">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H9" s="3">
         <f t="shared" si="2"/>
         <v>1.507556722888818</v>
       </c>
-      <c r="J9" s="3"/>
+      <c r="J9" s="3">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
@@ -971,18 +978,20 @@
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="3">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G10" s="16">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="G10" s="16">
-        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="H10" s="3">
         <f t="shared" si="2"/>
         <v>0.50251890762960605</v>
       </c>
-      <c r="J10" s="3"/>
+      <c r="J10" s="3">
+        <v>25</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -999,18 +1008,20 @@
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="3">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="G11" s="16">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="G11" s="16">
-        <f t="shared" si="1"/>
         <v>1.6666666666666667</v>
       </c>
       <c r="H11" s="3">
         <f t="shared" si="2"/>
         <v>0.50251890762960605</v>
       </c>
-      <c r="J11" s="3"/>
+      <c r="J11" s="3">
+        <v>25</v>
+      </c>
     </row>
     <row r="12" spans="1:10" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
@@ -1027,18 +1038,20 @@
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="3">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="G12" s="16">
         <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="G12" s="16">
-        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="H12" s="3">
         <f t="shared" si="2"/>
         <v>1.507556722888818</v>
       </c>
-      <c r="J12" s="3"/>
+      <c r="J12" s="3">
+        <v>70</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
@@ -1058,7 +1071,7 @@
         <v>3.6237153766973935</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1067,7 +1080,7 @@
         <v>422.75256924660522</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1076,13 +1089,22 @@
         <v>437.24743075339478</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
       <c r="H20">
-        <f>MEDIAN(H17, H18)/60</f>
-        <v>7.166666666666667</v>
+        <f>ROUND(MEDIAN(H17, H18)/60, 2)</f>
+        <v>7.17</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="J22">
+        <f>ROUND(SUM(J2:J12)/60, 2)</f>
+        <v>7.33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improve documentation and taskplan
</commit_message>
<xml_diff>
--- a/TaskPlan.xlsx
+++ b/TaskPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregoryseibert/Documents/dhbw-graphische-programmierung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB1A31DB-6ED8-EB46-9A0E-4CA919F4C523}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A19A8099-D4D0-E64C-B187-EF67FF461CF3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16180" xr2:uid="{B844A864-B968-094C-9F1D-B9ED8C2FA309}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16180" xr2:uid="{B844A864-B968-094C-9F1D-B9ED8C2FA309}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -681,10 +681,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78E6F04A-8579-EA48-AC2A-F124B89258CD}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,7 +771,7 @@
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="3">
-        <f t="shared" ref="F2:F12" si="1">(B3+4*C3+D3)/6</f>
+        <f t="shared" ref="F3:F12" si="1">(B3+4*C3+D3)/6</f>
         <v>45</v>
       </c>
       <c r="G3" s="16">
@@ -1109,5 +1112,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="64" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>